<commit_message>
added new data with new plunger
</commit_message>
<xml_diff>
--- a/data/commerical-Vs-printed-comparison/data-taking-raw/printed-pipette-300uL-160210.xlsx
+++ b/data/commerical-Vs-printed-comparison/data-taking-raw/printed-pipette-300uL-160210.xlsx
@@ -394,19 +394,19 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>283.5</v>
+        <v>298.8</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>286.2</v>
+        <v>296.8</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>285.2</v>
+        <v>296.7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -414,19 +414,19 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>285.60000000000002</v>
+        <v>299.7</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
-        <v>286.5</v>
+        <v>297.3</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
-        <v>286.8</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -434,19 +434,19 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>286</v>
+        <v>300.5</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4">
-        <v>285.3</v>
+        <v>297.89999999999998</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4">
-        <v>285.39999999999998</v>
+        <v>296.10000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -454,19 +454,19 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>285.5</v>
+        <v>300.10000000000002</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>287.2</v>
+        <v>297.8</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5">
-        <v>286.39999999999998</v>
+        <v>296.3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -474,19 +474,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>286.10000000000002</v>
+        <v>300.2</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6">
-        <v>284.89999999999998</v>
+        <v>297.8</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
       <c r="H6">
-        <v>286.7</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>